<commit_message>
1.update variety config; 2.fix download bug
</commit_message>
<xml_diff>
--- a/data/黑色金属合集.xlsx
+++ b/data/黑色金属合集.xlsx
@@ -40,7 +40,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t>yVjpCgZpNvOHlEoAN60+iXcNR8qcjD2afR3U+XlDrUTEX5W5KWYQZl2WlS6znR8JdtRv8fy9hcGzGgX1t8jwbDwAx0EUQZsw3ZWNu8RJYhGO4TcQ9l1JkQHbe3Y9+FG0Tmzb5nAqIClWWKfYkQKr3HY3DNkUELEitQOt11rUEoTIhVaMplO5MgbPDFX7usRnfVXDB/k4c7tZ47cmSdI5PPMsbpmHAPopJA7aC2nIqZViTl63R0xAiSk7Ri5cVjaz2ZfAsMKLU3YycgddTehBXHwhe9WPt2y69Y3ealJxW5FCNmoy/cvsfz4C6sen9IjSULD5tGWRee0KrXbw+QoZgE7NWEwsW6jdNhqSmrM452PxF17kzrO6bofpprYgvGEYh3rU3x+aGppWuK0MQKBbJADXdNV7+gERMXLgzr9hjufCSB2LcYeyCjF2BrBjkG6RO3w4OyoTaTxMFrdCERew7D8UQllfiPPcrDToYoxCMTTXw+yekHjb9H0taBNrfd9f70H6UBPeid3DIOEWH7OzCNa1BWH3ku7y2k3tmGXSjpLeG2fEhqT94ROjZdXU4nBy989wEKfH/8gCX8UfQHl3s4HNC5A/1jjfGVQXbKn5640M8CHZ0yBMaBAMB/IP8Dj27sRdi8bkRobqKGqrut7Oa8j0XGzrf3cRVi2O0Rl3ALkSWjfQFihpHhVpJ1vHF8R/0U5Jg02wXqeIxw4qzKns0CVxEaNAVhef1Nx8ROpLZkCyRQvuDu04RNlZF/DANR1FRmB3/ZoMviLQ1UGsJaWotgcAkEqFKn5GqNtfLi+HqGPs9oPjjnAWxibLAcjJ5ez+XjOha6FhoqrP7o6RDuBqzLs3RtKjAERPKCz6KeALMYdlh39rOD1/bd9sAlyS53/OloIhbmtmx9AAMhdHMCvAEtwRWQ33RSnQkh7mMEjo3wdoYO/DFdnsRbcO67lGLqVd8Q44SneH5zYW6I2LMPvmDOdJcEUYbvBcDJsD+C5E+O78YRvuTlOjLWZljMYY6RHKzJDrrtdP/JGUwWGOFHMgEl24qXwV9/9jKPd9xkux/tWJ4kV6to+li9dxCBkPplnW1b9zOHR8xSRqknhyT/HIcekOTjuQEWKpofz71lLd0CbumviQzcoMIwkFqVQsRnaTLtppix+XghE9BPxw5tYzvnupJWlzUIZ4jrVuRzUpIGRIw96qi9j+6IFIrRhBlG279abofzoTtP41tkjCxYwIWoxJkf02iRaY/eviAN4r/WSTcdq5G6DSY5Ff4CDPxL3tBmQOvU9PzJqbA55QNw1e7ZGduGHcclY4LXjOQi29bQIddimDq/KkfY/hAYZZvi5hQMT2QIByuRoJn+5NQdcqGH8ztRWpFKF6M2Qk63pZ0sjadGWAYm9zQzxTwXZjBoqYLTqhO1ZsE20pVnaUgTovRnur5zkZjL0Yyva67oppXfQ3nA0Qv3q/qS49AfNQCLielfDMEkxWa3v5Z1GbwQFGfZdESxYRT4rCJyGWNjPiiWfAjtjdxkGR4PiTwlks8N+FKMNYR8RDxWyDZzrUvDr1hjW4N1XNQt4E3aNdn8i/gawApuX5D/rrH7PMFJMYTbxJRhUopNk3FfhC9JMNDQMZT51dvtEP8DrbdX3l2zAo5PM/ytarE4wrq7aFmTZrD6lwDzAWWfXO/9mA+WoO6luRCZ9VU0XPj+RHvkEb/Aku+hfp4hw/ZPLxrdpEsUEC2gec01z+2eqU08pL9w64O4bqVDwd9Y/WPZl2uKhJ79pxRNcRYWNGswJS/o7zdTdqLi9yBTPeBPDzX0GDfBsobltiOTVjIIayYK0VoyjQ9/HylbvMwuvnAQV5BZFDiUappQtwde3viG1irlr5KCOUMZ1PGvkODAHw088kTmmNcTKhEe+0tEsI5lf0b86j2txQwmvuGUNjWebI7QO0+c+aLamNxG3MgL6huqeTJ5VjYjgVXMcXKoe84CPQ4wDYMMpRVFJGCAxCr8EH/F0bUNW7Ncq5W/ZWM04+BjVnV+JMb1V1esqXTAPoo1WBcPIHV5m9zdLNNkYxTEZmrVXPdstQkMSVhwTy3tLD1JRp2kr29Yc0PoIQV+zIXdvo+QWs9ClevC0yVMBo2uidHqyNzvuCpgRm9CRYO6Z9gPKdWu1dsP6+X76pAh9x1T77NOvTJ/c+NL8Mk+mTq+GB/ZUU6wRnYtJjoDx0oly1DyyXF+H4oCfZDGRF5FEhmb1i+johKMHTn0iAB/5AixOC3Pj7QKUoPMC2HpHDrM+Sv/lIotzKYoBJokYXImpq3LpRmqzMiw1JaU1h/GILcu3YGz2rKaMCXkjAhL+IeMEYG9nmbShPcKRBbnJb1yhcSbKg/uaG8Jzb8vS/lvVEqmDWsWgbpjYxAHuMVd/oRurxENyh+CDGx5RbiQkIxr93RwGWHOe8exSCwI/C70LP9zG5H756Mlw+EBdMjMhHGpW1b8oYgCL37sIAzXgwU0DENpNPLWOLDSSuZawmnFI4AA1NLRwUv3/XHd3gA96ujSzUMKem6m8o3d7G83MmXdGn/qgV0y9teFSXVNrI/adMZ3irARmJQ1mbMZZR/DUZ5oaBsuE7QMGqKF3bf1SLOxCYm55LkHU0S5v5YgQY9/nPZJ1CS2Zm1VPdMGjHrcqPdpqPwifP/AADknTKbXBsccj0zGeOemW/+oU4azJh5bVhgmlOtZ7LK5AsPTscW14pjXajvCnud9MnPnUZ+4eLLQt+fFnAoQKI/K+OSiO3mBkTLCdlcS1OXA928xhOfBZEy9Um/7Xq1lbsF3VhAV6fMQXLsPLUhz1PByJ2pLiurnLYc9Pir0kOYLm4qp9SDPKxacgq0PkKz9pJbbjaZRybwEkSRjMCMSuDuSVGnv+Dkln34sFjI7I7mti5/AXdJemjIfz8CU5gLnJTNYAc82bcnetIpldgt4+2RGY90TaDbwCPr874RMZFMd//qQoB9QTiLbPZX6I304FKiStCXDeg6vJ/H5K+Fv34/DaM0Hu7gAj9jvo38lTE2jmhSURW69oqxGl/U0J51K/ID87Ukc1Jg0izXrT6FEQk4BxU0QC7GnynrapRXC8SijhafEji9DHMfFfNpkCJKjiM0efSokJwEuGu6vRAttzukHAgOkS1EyYNRhatpBt6pFY/HjmLMZpngFydhJA8FGOxj5Nxzdpg5RA6+MidHSXiqtpwXtetIn4KPSdkYQbz/ijthdDQZORn4iIOTO6OtVvCxnjqSEQYpabCTnkE+95eT+Zd9wIBrRzGmBiQDS5oJeJCAMY9lw7g7IGHqlgyDdYccCEsKfDtzpPNPXArNyXxTqebBUx2JyJb1QiKIBwXRs+EiSQsG1rud/PoKvFkqT+14RTROwfhv7Y8yuDsheyLLDsv5wvCZIw7A5KhVJBnyWv9aTY4w43YG4zGQjV4+eQfhOJHp/8yiIDt+K+zCyOrrKftegMOWFtL3qDCIeVcCEs2QZfiNsedJSGgdZDuopa8yQbD1uh1K89d+J+6f0+FP8kv78i8hBDyfAYJqqjyhjWUVYLasoDXAIumiKrQK/XSd+T9ug2OltN4ZBpzujlRIEnVPfiz43rj9uORyIfbtmIAe5N6PITgjdi3GC/moWubwiwyAWTzRe5nfxC1/iCZ9cDccX1ItErBT9T+FbIofOnN1+c9Pe4lQTEcGOcvT72VfRrdZZZX0IvtFxkVr1G2Yv2ZqNbJqgHXwfxiBctxx3adC5DRkk8I1b1g+mbDMOp5UsFQmK42bVwHGyZbNQQMcjBxhGEnVnxSto1ORUGnzhudy8IN7RyBe4RTQzVFbk8iZdyypXHZgqjf/7ksXa6LB3GHNN9ksTb4WpB0LYMT+UaxSEO2i/iDC45ENLGHkpTdCzOBIFvkQOAT93mfzPmCPgYLJbiJrPMHTdzYoFOCNgucJxp9GwiNWXaSMk02Iz7Uc/eGYGUlQ1grlLA1GsstKXjBgGaJuILfTwhBDLUTZqja3nTsK2WLOpVkX9/QDkxbRpby1tJZ2CVcn4SqCHxHv8nlI6qBPfxpZz9dupGxIscYEPa9VUE7u/SRPZvV94f94y23npirSrs1rMnOFfYAiKphJWaxliQ/IP1tY4dVlBmv2O+1tCNPN0x4wZBhJxD5En0YJJtN7hBn96uvlIIlqgH2v2R9aWBeNw3ZB5KDS5UYYOjz6GguZp4HUXvtE9sRLzDQANVRR6fRpDLriGaYXhdNR27Sq/6jgu7mzaYuqQTck/egK3+KtHn0Mt+G5K4sgjIK8kLblgUfVUFmF2+dc96NKU3oQ+xe40qrEdpAY9V73p5gOnOEp11x2N93pb/H4u1mnV4i2tn63yMAujmceh/eAeE4e12d/fAowoKc+6v63XPkpY1TsDz76r2ZEXjWu7K6TJaOrjXzPQVOpY+S4j1i9V97Il6a0nSx50IRGxPBQASIP0IoPH0ATuyAVkPFy4RCQ9o+aI6n6mjJPBPnzokN5vK69M0ET7uBAEBpRFwH9fAMWFQzEiF4WFR/waeuyxj1nHMLBsCeYZ/OZBAaCR0OXqRM2omN1F+f+UqZf89WG18Log3m47hYRwJ/Bm8bPwkIjU6HGCNRU3chnBjUL7UFRR+wjLmYxE06gcg=</t>
+          <t>yVjpCgZpNvOHlEoAN60+iXcNR8qcjD2afR3U+XlDrUTEX5W5KWYQZl2WlS6znR8JdtRv8fy9hcGzGgX1t8jwbDwAx0EUQZsw3ZWNu8RJYhGO4TcQ9l1JkQHbe3Y9+FG0Tmzb5nAqIClWWKfYkQKr3HY3DNkUELEitQOt11rUEoTIhVaMplO5MgbPDFX7usRnfVXDB/k4c7tZ47cmSdI5PPMsbpmHAPopJA7aC2nIqZViTl63R0xAiSk7Ri5cVjaz2ZfAsMKLU3YycgddTehBXHwhe9WPt2y69Y3ealJxW5FCNmoy/cvsfz4C6sen9IjSULD5tGWRee0KrXbw+QoZgE7NWEwsW6jdNhqSmrM452PxF17kzrO6bofpprYgvGEYh3rU3x+aGppWuK0MQKBbJADXdNV7+gERMXLgzr9hjufCSB2LcYeyCjF2BrBjkG6RO3w4OyoTaTxMFrdCERew7D8UQllfiPPcrDToYoxCMTTXw+yekHjb9H0taBNrfd9f70H6UBPeid3DIOEWH7OzCNa1BWH3ku7y2k3tmGXSjpLeG2fEhqT94ROjZdXU4nBy989wEKfH/8gCX8UfQHl3s4HNC5A/1jjfGVQXbKn5640M8CHZ0yBMaBAMB/IP8Dj27sRdi8bkRobqKGqrut7Oa8j0XGzrf3cRVi2O0Rl3ALkSWjfQFihpHhVpJ1vHF8R/0U5Jg02wXqeIxw4qzKns0CVxEaNAVhef1Nx8ROpLZkCyRQvuDu04RNlZF/DANR1FRmB3/ZoMviLQ1UGsJaWotgcAkEqFKn5GqNtfLi+HqGPs9oPjjnAWxibLAcjJ5ez+XjOha6FhoqrP7o6RDuBqzLs3RtKjAERPKCz6KeALMYdlh39rOD1/bd9sAlyS53/OloIhbmtmx9AAMhdHMCvAEtwRWQ33RSnQkh7mMEjo3wdoYO/DFdnsRbcO67lGLqVd8Q44SneH5zYW6I2LMPvmDOdJcEUYbvBcDJsD+C5E+O78YRvuTlOjLWZljMYY6RHKzJDrrtdP/JGUwWGOFHMgEl24qXwV9/9jKPd9xkux/tWJ4kV6to+li9dxCBkPplnW1b9zOHR8xSRqknhyT/HIcekOTjuQEWKpofz71lLd0CbumviQzcoMIwkFqVQsRnaTLtppix+XghE9BPxw5tYzvnupJWlzUIZ4jrVuRzUpIGRIw96qi9j+6IFIrRhBlG279abofzoTtP41tkjCxYwIWoxJkf02iRaY/eviAN4r/WSTcdq5G6DSY5Ff4CDPxL3tBmQOvU9PzJqbA55QNw1e7ZGduGHcclY4LXjOQi29bQIddimDq/KkfY/hAYZZvi5hQMT2QIByuRoJn+5NQdcqGH8ztRWpFKF6M2Qk63pZ0sjadGWAYm9zQzxTwXZjBoqYLTqhO1ZsE20pVnaUgTovRnur5zkZjL0Yyva67oppXfQ3nA0Qv3q/qS49AfNQCLielfDMEkxWa3v5Z1GbwQFGfZdESxYRT4rCJyGWNjPiiWfAjtjdxkGR4PiTwlks8N+FKMNYR8RDxWyDZzrUvDr1hjW4N1XNQt4E3aNdn8i/gawApuX5D/rrH7PMFJMYTbxJRhUopNk3FfhC9JMNDQMZT51dvtEP8DrbdX3l2zAo5PM/ytarE4wrq7aFmTZrD6lwDzAWWfXO/9mA+WoO6luRCZ9VU0XPj+RHvkEb/Aku+hfp4hw/ZPLxrdpEsUEC2gec01z+2eqU08pL9w64O4bqVDwd9Y/WPZl2uKhJ79pxRNcRYWNGswJS/o7zdTdqLi9yBTPeBPDzX0GDfBsobltiOTVjIIayYK0VoyjQ9/HylbvMwuvnAQV5BZFDiUappQtwde3viG1irlr5KCOUMZ1PGvkODAHw088kTmmNcTKhEe+0tEsI5lf0b86j2txQwmvuGUNjWebI7QO0+c+aLamNxG3MgL6huqeTJ5VjYjgVXMcXKoe84CPQ4wDYMMpRVFJGCAxCr8EH/F0bUNW7Ncq5W/ZWM04+BjVnV+JMb1V1esqXTAPoo1WBcPIHV5m9zdLNNkYxTEZmrVXPdstQkMSVhwTy3tLD1JRp2kr29Yc0PoIQV+zIXdvo+QWs9ClevC0yVMBo2uidHqyNzvuCpgRm9CRYO6Z9gPKdWu1dsP6+X76pAh9x1T77NOvTJ/c+NL8Mk+mTq+GB/ZUU6wRnYtJjoDx0oly1DyyXF+H4oCfZDGRF5FEhmb1i+johKMHTn0iAB/5AixOC3Pj7QKUoPMC2HpHDrM+Sv/lIotzKYoBJokYXImpq3LpRmqzMiw1JaU1h/GILcu3YGz2rKaMCXkjAhL+IeMEYG9nmbShPcKRBbnJb1yhcSbKg/uaG8Jzb8vS/lvVEqmDWsWgbpjYxAHuMVd/oRurxENyh+CDGx5RbiQkIxr93RwGWHOe8exSCwI/C70LP9zG5H756Mlw+EBdMjMhHGpW1b8oYgCL37sIAzXgwU0DENpNPLWOLDSSuZawmnFI4AA1NLRwUv3/XHd3gA96ujSzUMKem6m8o3d7G83MmXdGn/qgV0y9teFSXVNrI/adMZ3irARmJQ1mbMZZR/DUZ5oaBsuE7QMGqKF3bf1SLOxCYm55LkHU0S5v5YgQY9/nPZJ1CS2Zm1VPdMGjHrcqPdpqPwifP/AADknTKbXBsccj0zGeOemW/+oU4azJh5bVhgmlOtZ7LK5AsPTscW14pjXajvCnud9MnPnUZ+4eLLQt+fFnAoQKI/K+OSiO3mBkTLCdlcS1OXA928xhOfBZEy9Um/7Xq1lbsF3VhAV6fMQXLsPLUhz1PByJ2pLiurnLYc9Pir0kOYLm4qp9SDPKxacgq0PkKz9pJbbjaZRybwEkSRjMCMSuDuSVGnv+Dkln34sFjI7I7mti5/AXdJemjIfz8CU5gLnJTNYAc82bcnetIpldgt4+2RGY90TaDbwCPr874RMZFMd//qQoB9QTiLbPZX6I304FKiStCXDeg6vJ/H5K+Fv34/DaM0Hu7gAj9jvo38lTE2jmhSURW69oqxGl/U0J51K/ID87Ukc1Jg0izXrT6FEQk4BxU0QC7GnynrapRXC8SijhafEji9DHMfFfNpkCJKjiM0efSokJwEuGu6vRAttzukHAgOkS1EyYNRhatpBt6pFY/HjmLMZpngFydhJA8FGOxj5Nxzdpg5RA6+MidHSXiqtpwXtetIn4KPSdkYQbz/ijthdDQZORn4iIOTO6OtVvCxnjqSEQYpabCTnkE+95eT+Zd9wIBrRzGmBiQDS5oJeJCAMY9lw7g7IGHqlgyDdYccCEsKfDtzpPNPXArNyXxTqebBUx2JyJb1QiKIBwXRs+EiSQsG1rud/PoKvFkqT+14RTROwfhv7Y8yuDsheyLLDsv5wvCZIw7A5KhVJBnyWv9aTY4w43YG4zGQjV4+eQfhOJHp/8yiIDt+K+zCyOrrKftegMOWFtL3qDCIeVcCEs2QZfiNsedJSGgdZDuopa8yQbD1uh1K89d+J+6f0+FP8kv78i8hBDyfAYJqqjyhjWUVYLasoDXAIumiKrQK/XSd+T9ug2OltN4ZBpzujlRIEnVPfiz43rj9uORyIfbtmIAe5N6PITgjdi3GC/moWubwiwyAWTzRe5nfxC1/iCZ9cDccX1ItErBT9T+FbIofOnN1+c9Pe4lQTEcGOcvT72VfRrdZZZX0IvtFxkVr1G2Yv2ZqNbJqgHXwfxiBctxx3adC5DRkk8I1b1g+mbDMOp5UsFQmK42bVwHGyZbNQQMcjBxhGEnVnxSto1ORUGnzhudy8IN7RyBe4RTQzVFbk8iZdyypXHZgqjf/7ksXa6LB3GHNN9ksTb4WpB0LYMT+UaxSEO2i/iDC45ENLGHkpTdCzOBIFvkQOAT93mfzPmCPgYLJbiJrPMHTdzYoFOCNgucJxp9GwiNWXaSMk02Iz7Uc/eGYGUlQ1grlLA1GsstKXjBgGaJuILfTwhBDLUTZqja3nTsK2WLOpVkX9/QDkxbRpby1tJZ2CVcn4SqCHxHv8nlI6qBPfxpZz9dupGxIscYEPa9VUE7u/SRPZvV94f94y23npirSrs1rMnOFfYAiKphJWaxliQ/IP1tY4dVlBmv2O+1tCNPN0x4wZBhJxD5En0YJJtN7hBn96uvlIIlqgH2v2R9aWBeNw3ZB5KDS5UYYOjz6GguZp4HUXvtE9sRLzDQANVRR6fRpDLriGaYXhdNR27Sq/6jgu7mzaYuqQTck/egK3+KtHn0Mt+G5K4sgjIK8kLblgUfVUFmF2+dc96NKU3oQ+xe40qrEdpAY9V73p5gOnOEp11x2N93pb/H4u1mnV4i2tn63yMAujmceh/eAeE4e12d/fAowoKc+6v63XPkpY1TsDz76r2ZEXjWu7K6TJaOrjXzPQVOpWcTgT8EtgsCW7HOEkpf++encv+JXzFdpY0rkSFlIWoPprrog52dbKNzPBN0akpfS3kDH7muUoPBEczmh24KbY0jM8kDmE/EP4Ovbke0vE16i3dkDpLs8Dsob2N9AKvN38YWfq3d2VtO5yuMrHmrnv4Fg8rnaRJDr129eufVIctdhqiaRWmLq9bEYkn/UqU7LmXVBXomvyN4Yf4BLzo9zss=</t>
         </r>
       </text>
     </comment>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="57">
   <si>
     <t>指标名称</t>
   </si>
@@ -159,46 +159,43 @@
     <t>2021-11-25~2024-06-13</t>
   </si>
   <si>
-    <t>2022-03-30~2024-06-05</t>
+    <t>2022-03-30~2024-06-12</t>
   </si>
   <si>
-    <t>2021-04-08~2024-06-04</t>
+    <t>2021-04-08~2024-06-19</t>
   </si>
   <si>
-    <t>2011-07-29~2024-06-12</t>
+    <t>2011-07-29~2024-06-19</t>
   </si>
   <si>
-    <t>2009-03-30~2024-06-13</t>
+    <t>2009-03-30~2024-06-19</t>
   </si>
   <si>
-    <t>2006-03-17~2024-06-07</t>
+    <t>2006-03-17~2024-06-14</t>
   </si>
   <si>
-    <t>2022-03-03~2024-06-06</t>
+    <t>2022-03-03~2024-06-13</t>
   </si>
   <si>
-    <t>2014-03-21~2024-06-13</t>
+    <t>2014-03-21~2024-06-19</t>
   </si>
   <si>
-    <t>2013-10-18~2024-06-12</t>
+    <t>2013-10-18~2024-06-19</t>
   </si>
   <si>
-    <t>2010-06-25~2024-06-07</t>
+    <t>2010-06-25~2024-06-14</t>
   </si>
   <si>
-    <t>2006-07-31~2024-06-06</t>
+    <t>2006-07-31~2024-06-13</t>
   </si>
   <si>
-    <t>2020-10-23~2024-06-07</t>
+    <t>2020-10-23~2024-06-14</t>
   </si>
   <si>
-    <t>2010-03-29~2024-06-12</t>
+    <t>2010-03-29~2024-06-19</t>
   </si>
   <si>
-    <t>2013-10-18~2024-06-13</t>
-  </si>
-  <si>
-    <t>2014-08-08~2024-06-13</t>
+    <t>2014-08-08~2024-06-19</t>
   </si>
   <si>
     <t>更新时间</t>
@@ -851,7 +848,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -859,6 +856,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1389,10 +1389,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:X4143"/>
+  <dimension ref="A1:X4147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1678,15 +1678,15 @@
         <v>47</v>
       </c>
       <c r="W5" t="s">
+        <v>43</v>
+      </c>
+      <c r="X5" t="s">
         <v>48</v>
-      </c>
-      <c r="X5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:24">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1">
         <v>45456</v>
@@ -1701,135 +1701,135 @@
         <v>45456</v>
       </c>
       <c r="F6" s="1">
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="G6" s="1">
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="H6" s="1">
-        <v>45447</v>
+        <v>45462</v>
       </c>
       <c r="I6" s="1">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="J6" s="1">
-        <v>45456</v>
+        <v>45462</v>
       </c>
       <c r="K6" s="1">
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="L6" s="1">
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="M6" s="1">
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="N6" s="1">
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="O6" s="1">
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="P6" s="1">
-        <v>45447</v>
+        <v>45462</v>
       </c>
       <c r="Q6" s="1">
-        <v>45456</v>
+        <v>45462</v>
       </c>
       <c r="R6" s="1">
-        <v>45455</v>
+        <v>45462</v>
       </c>
       <c r="S6" s="1">
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="T6" s="1">
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="U6" s="1">
-        <v>45450</v>
+        <v>45457</v>
       </c>
       <c r="V6" s="1">
-        <v>45456</v>
+        <v>45463</v>
       </c>
       <c r="W6" s="1">
-        <v>45456</v>
+        <v>45462</v>
       </c>
       <c r="X6" s="1">
-        <v>45456</v>
+        <v>45462</v>
       </c>
     </row>
     <row r="7" spans="1:24">
       <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" t="s">
         <v>52</v>
       </c>
-      <c r="C7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>53</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" t="s">
         <v>54</v>
       </c>
-      <c r="K7" t="s">
-        <v>52</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" t="s">
+        <v>54</v>
+      </c>
+      <c r="P7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>53</v>
+      </c>
+      <c r="R7" t="s">
         <v>55</v>
       </c>
-      <c r="M7" t="s">
-        <v>55</v>
-      </c>
-      <c r="N7" t="s">
-        <v>55</v>
-      </c>
-      <c r="O7" t="s">
-        <v>55</v>
-      </c>
-      <c r="P7" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>54</v>
-      </c>
-      <c r="R7" t="s">
-        <v>56</v>
-      </c>
       <c r="S7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="V7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="W7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -99409,6 +99409,9 @@
       <c r="G4135">
         <v>41.31</v>
       </c>
+      <c r="H4135">
+        <v>3764</v>
+      </c>
       <c r="I4135">
         <v>1912.9</v>
       </c>
@@ -99447,6 +99450,9 @@
       <c r="E4136">
         <v>231.14</v>
       </c>
+      <c r="H4136">
+        <v>3758</v>
+      </c>
       <c r="I4136">
         <v>1912.9</v>
       </c>
@@ -99464,6 +99470,9 @@
       </c>
       <c r="O4136">
         <v>60.88</v>
+      </c>
+      <c r="P4136">
+        <v>3864</v>
       </c>
       <c r="Q4136">
         <v>2758.2587</v>
@@ -99488,6 +99497,9 @@
       <c r="A4137" s="2">
         <v>45450</v>
       </c>
+      <c r="H4137">
+        <v>3767</v>
+      </c>
       <c r="I4137">
         <v>1912.9</v>
       </c>
@@ -99496,6 +99508,9 @@
       </c>
       <c r="K4137">
         <v>168.21</v>
+      </c>
+      <c r="P4137">
+        <v>3879</v>
       </c>
       <c r="Q4137">
         <v>2747.4505</v>
@@ -99523,11 +99538,17 @@
       <c r="A4138" s="2">
         <v>45454</v>
       </c>
+      <c r="H4138">
+        <v>3738</v>
+      </c>
       <c r="I4138">
         <v>1912.9</v>
       </c>
       <c r="J4138">
         <v>1318.4508</v>
+      </c>
+      <c r="P4138">
+        <v>3853</v>
       </c>
       <c r="Q4138">
         <v>2713.5847</v>
@@ -99549,11 +99570,23 @@
       <c r="A4139" s="2">
         <v>45455</v>
       </c>
+      <c r="F4139">
+        <v>50.95</v>
+      </c>
+      <c r="G4139">
+        <v>42.3</v>
+      </c>
+      <c r="H4139">
+        <v>3726</v>
+      </c>
       <c r="I4139">
         <v>1882.15</v>
       </c>
       <c r="J4139">
         <v>1322.4827</v>
+      </c>
+      <c r="P4139">
+        <v>3849</v>
       </c>
       <c r="Q4139">
         <v>2719.3491</v>
@@ -99587,12 +99620,42 @@
       <c r="E4140">
         <v>227.11</v>
       </c>
+      <c r="H4140">
+        <v>3727</v>
+      </c>
+      <c r="I4140">
+        <v>1874.15</v>
+      </c>
       <c r="J4140">
         <v>1327.2478</v>
       </c>
+      <c r="L4140">
+        <v>110.52</v>
+      </c>
+      <c r="M4140">
+        <v>93.17</v>
+      </c>
+      <c r="N4140">
+        <v>95.96</v>
+      </c>
+      <c r="O4140">
+        <v>60.63</v>
+      </c>
+      <c r="P4140">
+        <v>3848</v>
+      </c>
       <c r="Q4140">
         <v>2729.4368</v>
       </c>
+      <c r="R4140">
+        <v>825.89</v>
+      </c>
+      <c r="T4140">
+        <v>14894</v>
+      </c>
+      <c r="V4140">
+        <v>125.66</v>
+      </c>
       <c r="W4140">
         <v>6494.1248</v>
       </c>
@@ -99600,9 +99663,146 @@
         <v>2336.1033</v>
       </c>
     </row>
-    <row r="4143" spans="1:1">
-      <c r="A4143" s="3" t="s">
-        <v>57</v>
+    <row r="4141" spans="1:24">
+      <c r="A4141" s="2">
+        <v>45457</v>
+      </c>
+      <c r="H4141">
+        <v>3737</v>
+      </c>
+      <c r="I4141">
+        <v>1874.15</v>
+      </c>
+      <c r="J4141">
+        <v>1333.1124</v>
+      </c>
+      <c r="K4141">
+        <v>170.69</v>
+      </c>
+      <c r="P4141">
+        <v>3856</v>
+      </c>
+      <c r="Q4141">
+        <v>2742.4066</v>
+      </c>
+      <c r="R4141">
+        <v>840.67</v>
+      </c>
+      <c r="S4141">
+        <v>14075.52</v>
+      </c>
+      <c r="U4141">
+        <v>31.58</v>
+      </c>
+      <c r="V4141">
+        <v>125.16</v>
+      </c>
+      <c r="W4141">
+        <v>6577.5866</v>
+      </c>
+      <c r="X4141">
+        <v>2258.4703</v>
+      </c>
+    </row>
+    <row r="4142" spans="1:24">
+      <c r="A4142" s="2">
+        <v>45460</v>
+      </c>
+      <c r="H4142">
+        <v>3721</v>
+      </c>
+      <c r="I4142">
+        <v>1862.9</v>
+      </c>
+      <c r="J4142">
+        <v>1324.3154</v>
+      </c>
+      <c r="P4142">
+        <v>3843</v>
+      </c>
+      <c r="Q4142">
+        <v>2723.6724</v>
+      </c>
+      <c r="R4142">
+        <v>838.78</v>
+      </c>
+      <c r="V4142">
+        <v>126.84</v>
+      </c>
+      <c r="W4142">
+        <v>6462.3298</v>
+      </c>
+      <c r="X4142">
+        <v>2253.1367</v>
+      </c>
+    </row>
+    <row r="4143" spans="1:24">
+      <c r="A4143" s="3">
+        <v>45461</v>
+      </c>
+      <c r="H4143">
+        <v>3725</v>
+      </c>
+      <c r="I4143">
+        <v>1862.9</v>
+      </c>
+      <c r="J4143">
+        <v>1326.1481</v>
+      </c>
+      <c r="P4143">
+        <v>3848</v>
+      </c>
+      <c r="Q4143">
+        <v>2731.5984</v>
+      </c>
+      <c r="R4143">
+        <v>844.22</v>
+      </c>
+      <c r="V4143">
+        <v>126.24</v>
+      </c>
+      <c r="W4143">
+        <v>6521.9454</v>
+      </c>
+      <c r="X4143">
+        <v>2367.5121</v>
+      </c>
+    </row>
+    <row r="4144" spans="1:24">
+      <c r="A4144" s="2">
+        <v>45462</v>
+      </c>
+      <c r="H4144">
+        <v>3722</v>
+      </c>
+      <c r="I4144">
+        <v>1862.9</v>
+      </c>
+      <c r="J4144">
+        <v>1324.682</v>
+      </c>
+      <c r="P4144">
+        <v>3846</v>
+      </c>
+      <c r="Q4144">
+        <v>2727.9957</v>
+      </c>
+      <c r="R4144">
+        <v>847.11</v>
+      </c>
+      <c r="V4144">
+        <v>126.79</v>
+      </c>
+      <c r="W4144">
+        <v>6549.766</v>
+      </c>
+      <c r="X4144">
+        <v>2356.845</v>
+      </c>
+    </row>
+    <row r="4147" spans="1:1">
+      <c r="A4147" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>